<commit_message>
fix bug ，update side effect and Preparative regimens for hematopoietic cell transplantation
</commit_message>
<xml_diff>
--- a/data/side_effect.xlsx
+++ b/data/side_effect.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="118">
   <si>
     <t>药名</t>
   </si>
@@ -273,6 +273,9 @@
     <t>地西他滨</t>
   </si>
   <si>
+    <t xml:space="preserve"> Myelosuppression </t>
+  </si>
+  <si>
     <t>地塞米松(Dex)</t>
   </si>
   <si>
@@ -335,6 +338,10 @@
   </si>
   <si>
     <t>苯达莫司汀（Bendamustine）</t>
+  </si>
+  <si>
+    <t>These agents are markedly myelosuppressive, but with delayed effect,
+possibly up to 6 weeks. The use of these agents may also result in renal failure</t>
   </si>
   <si>
     <t>阿扎胞苷</t>
@@ -473,6 +480,9 @@
     <t>（或）氟达拉滨（FL）</t>
   </si>
   <si>
+    <t>fludarabine</t>
+  </si>
+  <si>
     <t>（C1之后）利妥昔单抗</t>
   </si>
   <si>
@@ -484,6 +494,39 @@
   </si>
   <si>
     <t>(optional)培门冬酶（PEG-ASP）</t>
+  </si>
+  <si>
+    <t>carmustine</t>
+  </si>
+  <si>
+    <t>TBI</t>
+  </si>
+  <si>
+    <t>Melphalan</t>
+  </si>
+  <si>
+    <t>busulfan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It produces adverse effects related to myelosuppression. It only
+occasionally produces nausea and vomiting. In high doses, it produces a rare but some-
+times fatal pulmonary fibrosis, “busulfan lung.” Its use is associated with adrenal insuf-
+ficiency and skin pigmentation.</t>
+  </si>
+  <si>
+    <t>thiotepa</t>
+  </si>
+  <si>
+    <t>Myelosuppression is a major toxicity.</t>
+  </si>
+  <si>
+    <t>nti-thymocyte globulin</t>
+  </si>
+  <si>
+    <t>Total lymphoid irradiation</t>
+  </si>
+  <si>
+    <t>cyclophosphamide</t>
   </si>
 </sst>
 </file>
@@ -491,12 +534,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,22 +560,14 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10.5"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -546,6 +581,127 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -554,120 +710,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Nimbus Roman No9 L"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -676,19 +725,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -700,7 +845,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -712,19 +857,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,132 +905,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -872,10 +927,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -898,16 +953,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -928,16 +998,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -953,17 +1023,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -972,152 +1036,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1141,6 +1205,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1461,10 +1531,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1777,12 +1847,14 @@
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="C34" s="1"/>
     </row>
     <row r="35" ht="57" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>22</v>
@@ -1791,7 +1863,7 @@
     </row>
     <row r="36" ht="57" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>22</v>
@@ -1800,19 +1872,19 @@
     </row>
     <row r="37" ht="120" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>33</v>
@@ -1820,96 +1892,98 @@
     </row>
     <row r="39" ht="71.25" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" ht="90" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" ht="90" spans="1:3">
       <c r="A41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" ht="45" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C42" s="1"/>
     </row>
     <row r="43" ht="135" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C43" s="1"/>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" ht="85.5" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
     <row r="47" ht="57" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row r="48" ht="57" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>33</v>
@@ -1917,30 +1991,30 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
     <row r="51" ht="90" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
     <row r="53" ht="75" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>50</v>
@@ -1949,7 +2023,7 @@
     </row>
     <row r="54" ht="165" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>4</v>
@@ -1958,25 +2032,25 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C55" s="1"/>
     </row>
     <row r="56" ht="15" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C56" s="1"/>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>8</v>
@@ -1985,7 +2059,7 @@
     </row>
     <row r="58" ht="57" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>22</v>
@@ -1994,7 +2068,7 @@
     </row>
     <row r="59" ht="57" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>56</v>
@@ -2003,16 +2077,16 @@
     </row>
     <row r="60" ht="57" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C60" s="1"/>
     </row>
     <row r="61" ht="75" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>47</v>
@@ -2021,7 +2095,7 @@
     </row>
     <row r="62" ht="57" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>56</v>
@@ -2030,61 +2104,125 @@
     </row>
     <row r="63" ht="95.25" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row r="64" ht="95.25" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" ht="15" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" ht="30" spans="1:3">
+    <row r="66" ht="15" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B66" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" ht="30" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="67" ht="45" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="68" ht="165" spans="1:3">
+    <row r="68" ht="45" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B68" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" ht="165" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="1"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" ht="85.5" spans="1:2">
+      <c r="A70" t="s">
+        <v>108</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="72" ht="57" spans="1:2">
+      <c r="A72" t="s">
+        <v>110</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" ht="156.75" spans="1:2">
+      <c r="A73" t="s">
+        <v>111</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" ht="15" spans="1:1">
+      <c r="A76" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" ht="75" spans="1:2">
+      <c r="A77" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>